<commit_message>
Added new WSJ survey (v1.03)
</commit_message>
<xml_diff>
--- a/modules/external-import/external-import-wsj.xlsx
+++ b/modules/external-import/external-import-wsj.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charles\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6776DB8F-6ADE-4370-B2AD-2853CE395C0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C7ED9E-3783-4ACF-923D-F2C376512517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{7EA91EED-77CB-43E4-BA35-3D98E29C29D5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{7EA91EED-77CB-43E4-BA35-3D98E29C29D5}"/>
   </bookViews>
   <sheets>
     <sheet name="wsj_2021-04-11" sheetId="6" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="wsj_2021-10-17" sheetId="1" r:id="rId3"/>
     <sheet name="wsj_2022-01-16" sheetId="2" r:id="rId4"/>
     <sheet name="wsj_2022-04-10" sheetId="7" r:id="rId5"/>
+    <sheet name="wsj_2022-07-17" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="107">
   <si>
     <t>2022Q1</t>
   </si>
@@ -353,6 +354,12 @@
   </si>
   <si>
     <t>S&amp;P Global Market Intelligence</t>
+  </si>
+  <si>
+    <t>EY-Parthenon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PNC Financial Services Group </t>
   </si>
 </sst>
 </file>
@@ -18795,7 +18802,7 @@
   <dimension ref="A1:AD76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24696,8 +24703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58E37947-8B93-4E68-9592-51DB3BAA2576}">
   <dimension ref="A1:AD78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30329,4 +30336,4837 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D2C548B-E808-471D-B491-E18D6AA7C3D0}">
+  <dimension ref="A1:Z78"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3">
+        <v>3.32</v>
+      </c>
+      <c r="C3">
+        <v>3.3</v>
+      </c>
+      <c r="D3">
+        <v>3.22</v>
+      </c>
+      <c r="E3">
+        <v>3.21</v>
+      </c>
+      <c r="F3">
+        <v>3.17</v>
+      </c>
+      <c r="G3">
+        <v>3.294</v>
+      </c>
+      <c r="H3">
+        <v>3.4660000000000002</v>
+      </c>
+      <c r="I3">
+        <v>3.282</v>
+      </c>
+      <c r="J3">
+        <v>2.9319999999999999</v>
+      </c>
+      <c r="K3">
+        <v>2.7559999999999998</v>
+      </c>
+      <c r="L3">
+        <v>0.37</v>
+      </c>
+      <c r="M3">
+        <v>1.5</v>
+      </c>
+      <c r="N3">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="O3">
+        <v>0.83</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>6.85</v>
+      </c>
+      <c r="R3">
+        <v>3.91</v>
+      </c>
+      <c r="S3">
+        <v>2.93</v>
+      </c>
+      <c r="T3">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="U3">
+        <v>2.31</v>
+      </c>
+      <c r="V3">
+        <v>3.76</v>
+      </c>
+      <c r="W3">
+        <v>4.05</v>
+      </c>
+      <c r="X3">
+        <v>4.28</v>
+      </c>
+      <c r="Y3">
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="Z3">
+        <v>4.3499999999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>2.87</v>
+      </c>
+      <c r="C4">
+        <v>2.59</v>
+      </c>
+      <c r="D4">
+        <v>2.54</v>
+      </c>
+      <c r="E4">
+        <v>2.54</v>
+      </c>
+      <c r="F4">
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="G4">
+        <v>3.375</v>
+      </c>
+      <c r="H4">
+        <v>3.375</v>
+      </c>
+      <c r="I4">
+        <v>3.375</v>
+      </c>
+      <c r="J4">
+        <v>2.875</v>
+      </c>
+      <c r="K4">
+        <v>2.375</v>
+      </c>
+      <c r="L4">
+        <v>3.3</v>
+      </c>
+      <c r="M4">
+        <v>1.4</v>
+      </c>
+      <c r="N4">
+        <v>1.8</v>
+      </c>
+      <c r="O4">
+        <v>1.3</v>
+      </c>
+      <c r="P4">
+        <v>1.2</v>
+      </c>
+      <c r="Q4">
+        <v>6.5</v>
+      </c>
+      <c r="R4">
+        <v>2.4</v>
+      </c>
+      <c r="S4">
+        <v>1.7</v>
+      </c>
+      <c r="T4">
+        <v>0.8</v>
+      </c>
+      <c r="U4">
+        <v>0.3</v>
+      </c>
+      <c r="V4">
+        <v>3.6</v>
+      </c>
+      <c r="W4">
+        <v>3.6</v>
+      </c>
+      <c r="X4">
+        <v>3.7</v>
+      </c>
+      <c r="Y4">
+        <v>3.7</v>
+      </c>
+      <c r="Z4">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>3.93</v>
+      </c>
+      <c r="C5">
+        <v>3.93</v>
+      </c>
+      <c r="D5">
+        <v>3.75</v>
+      </c>
+      <c r="E5">
+        <v>3.42</v>
+      </c>
+      <c r="F5">
+        <v>3.19</v>
+      </c>
+      <c r="G5">
+        <v>3.375</v>
+      </c>
+      <c r="H5">
+        <v>3.375</v>
+      </c>
+      <c r="I5">
+        <v>3.375</v>
+      </c>
+      <c r="J5">
+        <v>2.875</v>
+      </c>
+      <c r="K5">
+        <v>2.875</v>
+      </c>
+      <c r="L5">
+        <v>0.6</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>0.6</v>
+      </c>
+      <c r="O5">
+        <v>0.5</v>
+      </c>
+      <c r="P5">
+        <v>0.5</v>
+      </c>
+      <c r="Q5">
+        <v>7.4</v>
+      </c>
+      <c r="R5">
+        <v>4.5</v>
+      </c>
+      <c r="S5">
+        <v>3</v>
+      </c>
+      <c r="T5">
+        <v>2.5</v>
+      </c>
+      <c r="U5">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="V5">
+        <v>3.7</v>
+      </c>
+      <c r="W5">
+        <v>3.9</v>
+      </c>
+      <c r="X5">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="Y5">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="Z5">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>3.8</v>
+      </c>
+      <c r="C7">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D7">
+        <v>4.18</v>
+      </c>
+      <c r="E7">
+        <v>4.26</v>
+      </c>
+      <c r="F7">
+        <v>4.34</v>
+      </c>
+      <c r="G7">
+        <v>2.625</v>
+      </c>
+      <c r="H7">
+        <v>3.125</v>
+      </c>
+      <c r="I7">
+        <v>3.375</v>
+      </c>
+      <c r="J7">
+        <v>3.375</v>
+      </c>
+      <c r="K7">
+        <v>3.375</v>
+      </c>
+      <c r="L7">
+        <v>1.7</v>
+      </c>
+      <c r="M7">
+        <v>2.4</v>
+      </c>
+      <c r="N7">
+        <v>2.7</v>
+      </c>
+      <c r="O7">
+        <v>2.1</v>
+      </c>
+      <c r="P7">
+        <v>1.8</v>
+      </c>
+      <c r="Q7">
+        <v>6</v>
+      </c>
+      <c r="R7">
+        <v>2.4</v>
+      </c>
+      <c r="S7">
+        <v>1.8</v>
+      </c>
+      <c r="T7">
+        <v>1.9</v>
+      </c>
+      <c r="U7">
+        <v>2</v>
+      </c>
+      <c r="V7">
+        <v>3.6</v>
+      </c>
+      <c r="W7">
+        <v>3.6</v>
+      </c>
+      <c r="X7">
+        <v>3.5</v>
+      </c>
+      <c r="Y7">
+        <v>3.6</v>
+      </c>
+      <c r="Z7">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>2.9</v>
+      </c>
+      <c r="C8">
+        <v>2.8</v>
+      </c>
+      <c r="D8">
+        <v>3.1</v>
+      </c>
+      <c r="E8">
+        <v>3.1</v>
+      </c>
+      <c r="F8">
+        <v>3.25</v>
+      </c>
+      <c r="G8">
+        <v>2.88</v>
+      </c>
+      <c r="H8">
+        <v>2.88</v>
+      </c>
+      <c r="I8">
+        <v>2.38</v>
+      </c>
+      <c r="J8">
+        <v>2.38</v>
+      </c>
+      <c r="K8">
+        <v>2.38</v>
+      </c>
+      <c r="L8">
+        <v>0.3</v>
+      </c>
+      <c r="M8">
+        <v>1.5</v>
+      </c>
+      <c r="N8">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O8">
+        <v>-1.2</v>
+      </c>
+      <c r="P8">
+        <v>-0.2</v>
+      </c>
+      <c r="Q8">
+        <v>6.9</v>
+      </c>
+      <c r="R8">
+        <v>6.5</v>
+      </c>
+      <c r="S8">
+        <v>4.5</v>
+      </c>
+      <c r="T8">
+        <v>2.7</v>
+      </c>
+      <c r="U8">
+        <v>2.5</v>
+      </c>
+      <c r="V8">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="W8">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="X8">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="Y8">
+        <v>4.5</v>
+      </c>
+      <c r="Z8">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>3.45</v>
+      </c>
+      <c r="C9">
+        <v>3.65</v>
+      </c>
+      <c r="D9">
+        <v>3.35</v>
+      </c>
+      <c r="E9">
+        <v>3.25</v>
+      </c>
+      <c r="F9">
+        <v>3.1</v>
+      </c>
+      <c r="G9">
+        <v>3.375</v>
+      </c>
+      <c r="H9">
+        <v>3.625</v>
+      </c>
+      <c r="I9">
+        <v>3.375</v>
+      </c>
+      <c r="J9">
+        <v>3</v>
+      </c>
+      <c r="K9">
+        <v>2.75</v>
+      </c>
+      <c r="L9">
+        <v>-1.5</v>
+      </c>
+      <c r="M9">
+        <v>3.5</v>
+      </c>
+      <c r="N9">
+        <v>2</v>
+      </c>
+      <c r="O9">
+        <v>2</v>
+      </c>
+      <c r="P9">
+        <v>1.6</v>
+      </c>
+      <c r="Q9">
+        <v>6.5</v>
+      </c>
+      <c r="R9">
+        <v>3.5</v>
+      </c>
+      <c r="S9">
+        <v>2.8</v>
+      </c>
+      <c r="T9">
+        <v>2.6</v>
+      </c>
+      <c r="U9">
+        <v>2.5</v>
+      </c>
+      <c r="V9">
+        <v>3.7</v>
+      </c>
+      <c r="W9">
+        <v>3.8</v>
+      </c>
+      <c r="X9">
+        <v>3.9</v>
+      </c>
+      <c r="Y9">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="Z9">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>2.88</v>
+      </c>
+      <c r="C10">
+        <v>2.83</v>
+      </c>
+      <c r="D10">
+        <v>2.8</v>
+      </c>
+      <c r="G10">
+        <v>3.125</v>
+      </c>
+      <c r="H10">
+        <v>3.375</v>
+      </c>
+      <c r="I10">
+        <v>3.375</v>
+      </c>
+      <c r="L10">
+        <v>-2.1</v>
+      </c>
+      <c r="M10">
+        <v>1.5</v>
+      </c>
+      <c r="N10">
+        <v>1.8</v>
+      </c>
+      <c r="O10">
+        <v>1.8</v>
+      </c>
+      <c r="P10">
+        <v>1.9</v>
+      </c>
+      <c r="Q10">
+        <v>6.5</v>
+      </c>
+      <c r="R10">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="S10">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="V10">
+        <v>3.5</v>
+      </c>
+      <c r="W10">
+        <v>3.4</v>
+      </c>
+      <c r="X10">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11">
+        <v>3.65</v>
+      </c>
+      <c r="C11">
+        <v>3.55</v>
+      </c>
+      <c r="D11">
+        <v>3.25</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="F11">
+        <v>3</v>
+      </c>
+      <c r="G11">
+        <v>3.125</v>
+      </c>
+      <c r="H11">
+        <v>3.125</v>
+      </c>
+      <c r="I11">
+        <v>2.875</v>
+      </c>
+      <c r="J11">
+        <v>2.625</v>
+      </c>
+      <c r="K11">
+        <v>2.625</v>
+      </c>
+      <c r="L11">
+        <v>1.3</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>2</v>
+      </c>
+      <c r="O11">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="P11">
+        <v>2.7</v>
+      </c>
+      <c r="Q11">
+        <v>6.5</v>
+      </c>
+      <c r="R11">
+        <v>3</v>
+      </c>
+      <c r="S11">
+        <v>2.5</v>
+      </c>
+      <c r="T11">
+        <v>2</v>
+      </c>
+      <c r="U11">
+        <v>1.8</v>
+      </c>
+      <c r="V11">
+        <v>3.8</v>
+      </c>
+      <c r="W11">
+        <v>3.8</v>
+      </c>
+      <c r="X11">
+        <v>3.9</v>
+      </c>
+      <c r="Y11">
+        <v>3.9</v>
+      </c>
+      <c r="Z11">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>3.5</v>
+      </c>
+      <c r="C12">
+        <v>2.5</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>3.5</v>
+      </c>
+      <c r="F12">
+        <v>4</v>
+      </c>
+      <c r="G12">
+        <v>3.875</v>
+      </c>
+      <c r="H12">
+        <v>2.875</v>
+      </c>
+      <c r="I12">
+        <v>2.875</v>
+      </c>
+      <c r="J12">
+        <v>3.375</v>
+      </c>
+      <c r="K12">
+        <v>3.875</v>
+      </c>
+      <c r="L12">
+        <v>0.5</v>
+      </c>
+      <c r="M12">
+        <v>1.5</v>
+      </c>
+      <c r="N12">
+        <v>-1</v>
+      </c>
+      <c r="O12">
+        <v>1.5</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="R12">
+        <v>3.7</v>
+      </c>
+      <c r="S12">
+        <v>2.9</v>
+      </c>
+      <c r="T12">
+        <v>2.5</v>
+      </c>
+      <c r="U12">
+        <v>3</v>
+      </c>
+      <c r="V12">
+        <v>4.5</v>
+      </c>
+      <c r="W12">
+        <v>4.8</v>
+      </c>
+      <c r="X12">
+        <v>4.2</v>
+      </c>
+      <c r="Y12">
+        <v>4.2</v>
+      </c>
+      <c r="Z12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13">
+        <v>3.5</v>
+      </c>
+      <c r="C13">
+        <v>3.25</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>2.85</v>
+      </c>
+      <c r="F13">
+        <v>2.78</v>
+      </c>
+      <c r="G13">
+        <v>3.625</v>
+      </c>
+      <c r="H13">
+        <v>3.875</v>
+      </c>
+      <c r="I13">
+        <v>2.125</v>
+      </c>
+      <c r="J13">
+        <v>1.625</v>
+      </c>
+      <c r="K13">
+        <v>2</v>
+      </c>
+      <c r="L13">
+        <v>0.5</v>
+      </c>
+      <c r="M13">
+        <v>1.5</v>
+      </c>
+      <c r="N13">
+        <v>1.4</v>
+      </c>
+      <c r="O13">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P13">
+        <v>0.3</v>
+      </c>
+      <c r="Q13">
+        <v>6.8</v>
+      </c>
+      <c r="R13">
+        <v>2.7</v>
+      </c>
+      <c r="S13">
+        <v>1.6</v>
+      </c>
+      <c r="T13">
+        <v>2</v>
+      </c>
+      <c r="U13">
+        <v>2</v>
+      </c>
+      <c r="V13">
+        <v>3.5</v>
+      </c>
+      <c r="W13">
+        <v>3.6</v>
+      </c>
+      <c r="X13">
+        <v>3.7</v>
+      </c>
+      <c r="Y13">
+        <v>3.8</v>
+      </c>
+      <c r="Z13">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14">
+        <v>3.1</v>
+      </c>
+      <c r="C14">
+        <v>3.1</v>
+      </c>
+      <c r="D14">
+        <v>3.2</v>
+      </c>
+      <c r="E14">
+        <v>3.3</v>
+      </c>
+      <c r="F14">
+        <v>3.3</v>
+      </c>
+      <c r="G14">
+        <v>3.125</v>
+      </c>
+      <c r="H14">
+        <v>3.375</v>
+      </c>
+      <c r="I14">
+        <v>3.625</v>
+      </c>
+      <c r="J14">
+        <v>3.375</v>
+      </c>
+      <c r="K14">
+        <v>3.125</v>
+      </c>
+      <c r="L14">
+        <v>1.3</v>
+      </c>
+      <c r="M14">
+        <v>2</v>
+      </c>
+      <c r="N14">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="O14">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P14">
+        <v>0.9</v>
+      </c>
+      <c r="Q14">
+        <v>6.5</v>
+      </c>
+      <c r="R14">
+        <v>3.4</v>
+      </c>
+      <c r="S14">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="T14">
+        <v>1.8</v>
+      </c>
+      <c r="U14">
+        <v>1.6</v>
+      </c>
+      <c r="V14">
+        <v>3.7</v>
+      </c>
+      <c r="W14">
+        <v>4</v>
+      </c>
+      <c r="X14">
+        <v>4.3</v>
+      </c>
+      <c r="Y14">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="Z14">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15">
+        <v>3.25</v>
+      </c>
+      <c r="C15">
+        <v>3.1</v>
+      </c>
+      <c r="D15">
+        <v>3</v>
+      </c>
+      <c r="E15">
+        <v>2.75</v>
+      </c>
+      <c r="F15">
+        <v>2.5</v>
+      </c>
+      <c r="G15">
+        <v>3.375</v>
+      </c>
+      <c r="H15">
+        <v>3.375</v>
+      </c>
+      <c r="I15">
+        <v>2.875</v>
+      </c>
+      <c r="J15">
+        <v>2.375</v>
+      </c>
+      <c r="K15">
+        <v>1.625</v>
+      </c>
+      <c r="L15">
+        <v>0.7</v>
+      </c>
+      <c r="M15">
+        <v>1.4</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+      <c r="O15">
+        <v>-0.9</v>
+      </c>
+      <c r="P15">
+        <v>-0.5</v>
+      </c>
+      <c r="Q15">
+        <v>7</v>
+      </c>
+      <c r="R15">
+        <v>3.8</v>
+      </c>
+      <c r="S15">
+        <v>2.9</v>
+      </c>
+      <c r="T15">
+        <v>2.6</v>
+      </c>
+      <c r="U15">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="V15">
+        <v>3.6</v>
+      </c>
+      <c r="W15">
+        <v>3.7</v>
+      </c>
+      <c r="X15">
+        <v>3.9</v>
+      </c>
+      <c r="Y15">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="Z15">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16">
+        <v>3.8</v>
+      </c>
+      <c r="C16">
+        <v>3.6</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="G16">
+        <v>3.875</v>
+      </c>
+      <c r="H16">
+        <v>4.375</v>
+      </c>
+      <c r="I16">
+        <v>3.875</v>
+      </c>
+      <c r="L16">
+        <v>3.5</v>
+      </c>
+      <c r="M16">
+        <v>1.7</v>
+      </c>
+      <c r="N16">
+        <v>0.8</v>
+      </c>
+      <c r="O16">
+        <v>0.3</v>
+      </c>
+      <c r="P16">
+        <v>-2</v>
+      </c>
+      <c r="Q16">
+        <v>8.5</v>
+      </c>
+      <c r="R16">
+        <v>4.5</v>
+      </c>
+      <c r="S16">
+        <v>2</v>
+      </c>
+      <c r="V16">
+        <v>3.5</v>
+      </c>
+      <c r="W16">
+        <v>3.9</v>
+      </c>
+      <c r="X16">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17">
+        <v>3.2</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17">
+        <v>2.5</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17">
+        <v>2.5</v>
+      </c>
+      <c r="G17">
+        <v>3.1</v>
+      </c>
+      <c r="H17">
+        <v>3</v>
+      </c>
+      <c r="I17">
+        <v>2.75</v>
+      </c>
+      <c r="J17">
+        <v>2.5</v>
+      </c>
+      <c r="K17">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>1.5</v>
+      </c>
+      <c r="N17">
+        <v>1.5</v>
+      </c>
+      <c r="O17">
+        <v>1</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>7.5</v>
+      </c>
+      <c r="R17">
+        <v>5.5</v>
+      </c>
+      <c r="S17">
+        <v>3.4</v>
+      </c>
+      <c r="T17">
+        <v>2.5</v>
+      </c>
+      <c r="U17">
+        <v>2.5</v>
+      </c>
+      <c r="V17">
+        <v>3.7</v>
+      </c>
+      <c r="W17">
+        <v>4</v>
+      </c>
+      <c r="X17">
+        <v>4.3</v>
+      </c>
+      <c r="Y17">
+        <v>4.5</v>
+      </c>
+      <c r="Z17">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18">
+        <v>3.4</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>2.8</v>
+      </c>
+      <c r="E18">
+        <v>2.7</v>
+      </c>
+      <c r="F18">
+        <v>2.5</v>
+      </c>
+      <c r="G18">
+        <v>3.375</v>
+      </c>
+      <c r="H18">
+        <v>3.875</v>
+      </c>
+      <c r="I18">
+        <v>3.875</v>
+      </c>
+      <c r="J18">
+        <v>3.375</v>
+      </c>
+      <c r="K18">
+        <v>2.875</v>
+      </c>
+      <c r="L18">
+        <v>0.5</v>
+      </c>
+      <c r="M18">
+        <v>1.5</v>
+      </c>
+      <c r="N18">
+        <v>0.5</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>1</v>
+      </c>
+      <c r="Q18">
+        <v>6.9</v>
+      </c>
+      <c r="R18">
+        <v>3.6</v>
+      </c>
+      <c r="S18">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="T18">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="U18">
+        <v>2.5</v>
+      </c>
+      <c r="V18">
+        <v>3.8</v>
+      </c>
+      <c r="W18">
+        <v>4.2</v>
+      </c>
+      <c r="X18">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="Y18">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="Z18">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>72</v>
+      </c>
+      <c r="G19">
+        <v>3.625</v>
+      </c>
+      <c r="H19">
+        <v>3.875</v>
+      </c>
+      <c r="I19">
+        <v>3.875</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>2.5</v>
+      </c>
+      <c r="N19">
+        <v>2.4</v>
+      </c>
+      <c r="O19">
+        <v>0.9</v>
+      </c>
+      <c r="P19">
+        <v>0.9</v>
+      </c>
+      <c r="Q19">
+        <v>7.9</v>
+      </c>
+      <c r="R19">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="S19">
+        <v>2.8</v>
+      </c>
+      <c r="V19">
+        <v>3.5</v>
+      </c>
+      <c r="W19">
+        <v>3.6</v>
+      </c>
+      <c r="X19">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20">
+        <v>3.1</v>
+      </c>
+      <c r="C20">
+        <v>3.1</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="G20">
+        <v>3.375</v>
+      </c>
+      <c r="H20">
+        <v>3.875</v>
+      </c>
+      <c r="I20">
+        <v>3.875</v>
+      </c>
+      <c r="L20">
+        <v>1.3</v>
+      </c>
+      <c r="M20">
+        <v>1.5</v>
+      </c>
+      <c r="N20">
+        <v>1.5</v>
+      </c>
+      <c r="O20">
+        <v>1.5</v>
+      </c>
+      <c r="P20">
+        <v>1.5</v>
+      </c>
+      <c r="Q20">
+        <v>6.9</v>
+      </c>
+      <c r="R20">
+        <v>3.2</v>
+      </c>
+      <c r="S20">
+        <v>2</v>
+      </c>
+      <c r="V20">
+        <v>3.5</v>
+      </c>
+      <c r="W20">
+        <v>3.5</v>
+      </c>
+      <c r="X20">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21">
+        <v>3.1</v>
+      </c>
+      <c r="C21">
+        <v>3.2</v>
+      </c>
+      <c r="D21">
+        <v>2.7</v>
+      </c>
+      <c r="E21">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F21">
+        <v>2</v>
+      </c>
+      <c r="G21">
+        <v>2.875</v>
+      </c>
+      <c r="H21">
+        <v>2.875</v>
+      </c>
+      <c r="I21">
+        <v>2.125</v>
+      </c>
+      <c r="J21">
+        <v>1.625</v>
+      </c>
+      <c r="K21">
+        <v>1.625</v>
+      </c>
+      <c r="L21">
+        <v>-1.5</v>
+      </c>
+      <c r="M21">
+        <v>-2</v>
+      </c>
+      <c r="N21">
+        <v>-2.5</v>
+      </c>
+      <c r="O21">
+        <v>-1</v>
+      </c>
+      <c r="P21">
+        <v>-1</v>
+      </c>
+      <c r="Q21">
+        <v>7.2</v>
+      </c>
+      <c r="R21">
+        <v>6.3</v>
+      </c>
+      <c r="S21">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="T21">
+        <v>3.5</v>
+      </c>
+      <c r="U21">
+        <v>3</v>
+      </c>
+      <c r="V21">
+        <v>4</v>
+      </c>
+      <c r="W21">
+        <v>4.8</v>
+      </c>
+      <c r="X21">
+        <v>5.3</v>
+      </c>
+      <c r="Y21">
+        <v>5</v>
+      </c>
+      <c r="Z21">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>105</v>
+      </c>
+      <c r="B22">
+        <v>3.05</v>
+      </c>
+      <c r="C22">
+        <v>2.88</v>
+      </c>
+      <c r="D22">
+        <v>2.67</v>
+      </c>
+      <c r="E22">
+        <v>2.62</v>
+      </c>
+      <c r="F22">
+        <v>2.65</v>
+      </c>
+      <c r="G22">
+        <v>3.38</v>
+      </c>
+      <c r="H22">
+        <v>3.13</v>
+      </c>
+      <c r="I22">
+        <v>2.63</v>
+      </c>
+      <c r="J22">
+        <v>2.38</v>
+      </c>
+      <c r="K22">
+        <v>2.38</v>
+      </c>
+      <c r="L22">
+        <v>-1</v>
+      </c>
+      <c r="M22">
+        <v>1.9</v>
+      </c>
+      <c r="N22">
+        <v>-0.5</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>1.4</v>
+      </c>
+      <c r="Q22">
+        <v>6.1</v>
+      </c>
+      <c r="R22">
+        <v>2.1</v>
+      </c>
+      <c r="S22">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="T22">
+        <v>1.4</v>
+      </c>
+      <c r="U22">
+        <v>2.1</v>
+      </c>
+      <c r="V22">
+        <v>4</v>
+      </c>
+      <c r="W22">
+        <v>4.8</v>
+      </c>
+      <c r="X22">
+        <v>4.8</v>
+      </c>
+      <c r="Y22">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="Z22">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23">
+        <v>3.77</v>
+      </c>
+      <c r="C23">
+        <v>4.33</v>
+      </c>
+      <c r="D23">
+        <v>3.96</v>
+      </c>
+      <c r="E23">
+        <v>3.69</v>
+      </c>
+      <c r="F23">
+        <v>3.57</v>
+      </c>
+      <c r="G23">
+        <v>3.625</v>
+      </c>
+      <c r="H23">
+        <v>3.375</v>
+      </c>
+      <c r="I23">
+        <v>3.125</v>
+      </c>
+      <c r="J23">
+        <v>2.875</v>
+      </c>
+      <c r="K23">
+        <v>2.875</v>
+      </c>
+      <c r="L23">
+        <v>1</v>
+      </c>
+      <c r="M23">
+        <v>0.5</v>
+      </c>
+      <c r="N23">
+        <v>0.9</v>
+      </c>
+      <c r="O23">
+        <v>1</v>
+      </c>
+      <c r="P23">
+        <v>1.5</v>
+      </c>
+      <c r="Q23">
+        <v>6.8</v>
+      </c>
+      <c r="R23">
+        <v>3.6</v>
+      </c>
+      <c r="S23">
+        <v>2.7</v>
+      </c>
+      <c r="T23">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="U23">
+        <v>1.8</v>
+      </c>
+      <c r="V23">
+        <v>4.3</v>
+      </c>
+      <c r="W23">
+        <v>4.7</v>
+      </c>
+      <c r="X23">
+        <v>5</v>
+      </c>
+      <c r="Y23">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="Z23">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24">
+        <v>3.45</v>
+      </c>
+      <c r="C24">
+        <v>3.6</v>
+      </c>
+      <c r="D24">
+        <v>3.7</v>
+      </c>
+      <c r="E24">
+        <v>3.65</v>
+      </c>
+      <c r="F24">
+        <v>3.6</v>
+      </c>
+      <c r="G24">
+        <v>3.25</v>
+      </c>
+      <c r="H24">
+        <v>3.5</v>
+      </c>
+      <c r="L24">
+        <v>-1.8</v>
+      </c>
+      <c r="M24">
+        <v>0.4</v>
+      </c>
+      <c r="N24">
+        <v>0.3</v>
+      </c>
+      <c r="O24">
+        <v>-0.6</v>
+      </c>
+      <c r="P24">
+        <v>-0.2</v>
+      </c>
+      <c r="Q24">
+        <v>7.7</v>
+      </c>
+      <c r="S24">
+        <v>3.2</v>
+      </c>
+      <c r="U24">
+        <v>1.4</v>
+      </c>
+      <c r="V24">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="W24">
+        <v>5</v>
+      </c>
+      <c r="X24">
+        <v>5.9</v>
+      </c>
+      <c r="Y24">
+        <v>6.5</v>
+      </c>
+      <c r="Z24">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25">
+        <v>3.7</v>
+      </c>
+      <c r="C25">
+        <v>3.6</v>
+      </c>
+      <c r="D25">
+        <v>2.8</v>
+      </c>
+      <c r="E25">
+        <v>2.7</v>
+      </c>
+      <c r="F25">
+        <v>2.7</v>
+      </c>
+      <c r="G25">
+        <v>3.625</v>
+      </c>
+      <c r="H25">
+        <v>3.875</v>
+      </c>
+      <c r="I25">
+        <v>3.375</v>
+      </c>
+      <c r="J25">
+        <v>2.625</v>
+      </c>
+      <c r="K25">
+        <v>2.625</v>
+      </c>
+      <c r="L25">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M25">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="N25">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O25">
+        <v>0.6</v>
+      </c>
+      <c r="P25">
+        <v>0.8</v>
+      </c>
+      <c r="Q25">
+        <v>8.1</v>
+      </c>
+      <c r="R25">
+        <v>3.6</v>
+      </c>
+      <c r="S25">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="T25">
+        <v>2</v>
+      </c>
+      <c r="U25">
+        <v>2</v>
+      </c>
+      <c r="V25">
+        <v>4</v>
+      </c>
+      <c r="W25">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="X25">
+        <v>5</v>
+      </c>
+      <c r="Y25">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="Z25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26">
+        <v>3</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+      <c r="D26">
+        <v>3.02</v>
+      </c>
+      <c r="G26">
+        <v>3.375</v>
+      </c>
+      <c r="H26">
+        <v>2.6749999999999998</v>
+      </c>
+      <c r="I26">
+        <v>3.125</v>
+      </c>
+      <c r="L26">
+        <v>-1.4</v>
+      </c>
+      <c r="M26">
+        <v>1.8</v>
+      </c>
+      <c r="N26">
+        <v>1.6</v>
+      </c>
+      <c r="O26">
+        <v>-0.4</v>
+      </c>
+      <c r="P26">
+        <v>-1.3</v>
+      </c>
+      <c r="Q26">
+        <v>5.7</v>
+      </c>
+      <c r="R26">
+        <v>1.8</v>
+      </c>
+      <c r="S26">
+        <v>1.6</v>
+      </c>
+      <c r="V26">
+        <v>3.7</v>
+      </c>
+      <c r="W26">
+        <v>4.5</v>
+      </c>
+      <c r="X26">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>106</v>
+      </c>
+      <c r="B27">
+        <v>3.22</v>
+      </c>
+      <c r="C27">
+        <v>3.28</v>
+      </c>
+      <c r="D27">
+        <v>3.23</v>
+      </c>
+      <c r="E27">
+        <v>3.12</v>
+      </c>
+      <c r="F27">
+        <v>3.09</v>
+      </c>
+      <c r="G27">
+        <v>3.375</v>
+      </c>
+      <c r="H27">
+        <v>3.625</v>
+      </c>
+      <c r="I27">
+        <v>3.375</v>
+      </c>
+      <c r="J27">
+        <v>2.625</v>
+      </c>
+      <c r="K27">
+        <v>2.625</v>
+      </c>
+      <c r="L27">
+        <v>2</v>
+      </c>
+      <c r="M27">
+        <v>2.5</v>
+      </c>
+      <c r="N27">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O27">
+        <v>0.8</v>
+      </c>
+      <c r="P27">
+        <v>0.8</v>
+      </c>
+      <c r="Q27">
+        <v>5.2</v>
+      </c>
+      <c r="R27">
+        <v>3.2</v>
+      </c>
+      <c r="S27">
+        <v>2.4</v>
+      </c>
+      <c r="T27">
+        <v>2.1</v>
+      </c>
+      <c r="U27">
+        <v>2</v>
+      </c>
+      <c r="V27">
+        <v>3.7</v>
+      </c>
+      <c r="W27">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="X27">
+        <v>4.2</v>
+      </c>
+      <c r="Y27">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="Z27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28">
+        <v>3.3</v>
+      </c>
+      <c r="C28">
+        <v>3.4</v>
+      </c>
+      <c r="D28">
+        <v>3.5</v>
+      </c>
+      <c r="E28">
+        <v>3.4</v>
+      </c>
+      <c r="F28">
+        <v>3.3</v>
+      </c>
+      <c r="G28">
+        <v>3.125</v>
+      </c>
+      <c r="H28">
+        <v>3.625</v>
+      </c>
+      <c r="I28">
+        <v>3.875</v>
+      </c>
+      <c r="J28">
+        <v>3.625</v>
+      </c>
+      <c r="K28">
+        <v>3.375</v>
+      </c>
+      <c r="L28">
+        <v>0.7</v>
+      </c>
+      <c r="M28">
+        <v>-1.3</v>
+      </c>
+      <c r="N28">
+        <v>-0.9</v>
+      </c>
+      <c r="O28">
+        <v>0.8</v>
+      </c>
+      <c r="P28">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Q28">
+        <v>7.4</v>
+      </c>
+      <c r="R28">
+        <v>3.9</v>
+      </c>
+      <c r="S28">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="T28">
+        <v>2.1</v>
+      </c>
+      <c r="U28">
+        <v>2.4</v>
+      </c>
+      <c r="V28">
+        <v>3.9</v>
+      </c>
+      <c r="W28">
+        <v>4.3</v>
+      </c>
+      <c r="X28">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="Y28">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="Z28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>33</v>
+      </c>
+      <c r="B29">
+        <v>4.3899999999999997</v>
+      </c>
+      <c r="C29">
+        <v>4.33</v>
+      </c>
+      <c r="D29">
+        <v>4.3</v>
+      </c>
+      <c r="G29">
+        <v>3.125</v>
+      </c>
+      <c r="H29">
+        <v>3.125</v>
+      </c>
+      <c r="I29">
+        <v>3.125</v>
+      </c>
+      <c r="L29">
+        <v>0.5</v>
+      </c>
+      <c r="M29">
+        <v>1.6</v>
+      </c>
+      <c r="N29">
+        <v>1.5</v>
+      </c>
+      <c r="O29">
+        <v>1.5</v>
+      </c>
+      <c r="P29">
+        <v>1.5</v>
+      </c>
+      <c r="Q29">
+        <v>9.1</v>
+      </c>
+      <c r="R29">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="S29">
+        <v>3.8</v>
+      </c>
+      <c r="V29">
+        <v>3.5</v>
+      </c>
+      <c r="W29">
+        <v>3.4</v>
+      </c>
+      <c r="X29">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30">
+        <v>2.9</v>
+      </c>
+      <c r="C30">
+        <v>2.9</v>
+      </c>
+      <c r="D30">
+        <v>2.9</v>
+      </c>
+      <c r="E30">
+        <v>2.8</v>
+      </c>
+      <c r="F30">
+        <v>2.8</v>
+      </c>
+      <c r="G30">
+        <v>3.375</v>
+      </c>
+      <c r="H30">
+        <v>3.8250000000000002</v>
+      </c>
+      <c r="I30">
+        <v>3.8250000000000002</v>
+      </c>
+      <c r="J30">
+        <v>3.375</v>
+      </c>
+      <c r="K30">
+        <v>2.8250000000000002</v>
+      </c>
+      <c r="L30">
+        <v>1.5</v>
+      </c>
+      <c r="M30">
+        <v>2</v>
+      </c>
+      <c r="N30">
+        <v>1.9</v>
+      </c>
+      <c r="O30">
+        <v>1.5</v>
+      </c>
+      <c r="P30">
+        <v>1.5</v>
+      </c>
+      <c r="Q30">
+        <v>5.4</v>
+      </c>
+      <c r="R30">
+        <v>3</v>
+      </c>
+      <c r="S30">
+        <v>2.7</v>
+      </c>
+      <c r="T30">
+        <v>2.4</v>
+      </c>
+      <c r="U30">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="V30">
+        <v>3.7</v>
+      </c>
+      <c r="W30">
+        <v>3.9</v>
+      </c>
+      <c r="X30">
+        <v>4.3</v>
+      </c>
+      <c r="Y30">
+        <v>4.5</v>
+      </c>
+      <c r="Z30">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31">
+        <v>3.2</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31">
+        <v>1.8</v>
+      </c>
+      <c r="E31">
+        <v>2.4</v>
+      </c>
+      <c r="F31">
+        <v>3</v>
+      </c>
+      <c r="G31">
+        <v>3.375</v>
+      </c>
+      <c r="H31">
+        <v>2.375</v>
+      </c>
+      <c r="I31">
+        <v>1.375</v>
+      </c>
+      <c r="J31">
+        <v>1.875</v>
+      </c>
+      <c r="K31">
+        <v>2.375</v>
+      </c>
+      <c r="L31">
+        <v>1</v>
+      </c>
+      <c r="M31">
+        <v>1</v>
+      </c>
+      <c r="N31">
+        <v>0.5</v>
+      </c>
+      <c r="O31">
+        <v>-1</v>
+      </c>
+      <c r="P31">
+        <v>-1.5</v>
+      </c>
+      <c r="Q31">
+        <v>7.7</v>
+      </c>
+      <c r="R31">
+        <v>4.8</v>
+      </c>
+      <c r="S31">
+        <v>3.1</v>
+      </c>
+      <c r="T31">
+        <v>2.4</v>
+      </c>
+      <c r="U31">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="V31">
+        <v>3.6</v>
+      </c>
+      <c r="W31">
+        <v>4.8</v>
+      </c>
+      <c r="X31">
+        <v>4.5</v>
+      </c>
+      <c r="Y31">
+        <v>3.7</v>
+      </c>
+      <c r="Z31">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32">
+        <v>2.8</v>
+      </c>
+      <c r="C32">
+        <v>2.65</v>
+      </c>
+      <c r="D32">
+        <v>2.6</v>
+      </c>
+      <c r="E32">
+        <v>2.25</v>
+      </c>
+      <c r="F32">
+        <v>2.25</v>
+      </c>
+      <c r="G32">
+        <v>3.125</v>
+      </c>
+      <c r="H32">
+        <v>3.375</v>
+      </c>
+      <c r="I32">
+        <v>3.375</v>
+      </c>
+      <c r="J32">
+        <v>2.625</v>
+      </c>
+      <c r="K32">
+        <v>2.125</v>
+      </c>
+      <c r="L32">
+        <v>0.6</v>
+      </c>
+      <c r="M32">
+        <v>1</v>
+      </c>
+      <c r="N32">
+        <v>1.3</v>
+      </c>
+      <c r="O32">
+        <v>1.5</v>
+      </c>
+      <c r="P32">
+        <v>1.9</v>
+      </c>
+      <c r="Q32">
+        <v>7.6</v>
+      </c>
+      <c r="R32">
+        <v>4</v>
+      </c>
+      <c r="S32">
+        <v>3.1</v>
+      </c>
+      <c r="T32">
+        <v>3</v>
+      </c>
+      <c r="U32">
+        <v>2.8</v>
+      </c>
+      <c r="V32">
+        <v>3.4</v>
+      </c>
+      <c r="W32">
+        <v>3.4</v>
+      </c>
+      <c r="X32">
+        <v>3.7</v>
+      </c>
+      <c r="Y32">
+        <v>3.7</v>
+      </c>
+      <c r="Z32">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>103</v>
+      </c>
+      <c r="B33">
+        <v>3.5</v>
+      </c>
+      <c r="C33">
+        <v>3.3</v>
+      </c>
+      <c r="D33">
+        <v>3.25</v>
+      </c>
+      <c r="G33">
+        <v>3.375</v>
+      </c>
+      <c r="H33">
+        <v>3.375</v>
+      </c>
+      <c r="I33">
+        <v>2.875</v>
+      </c>
+      <c r="J33">
+        <v>2.375</v>
+      </c>
+      <c r="L33">
+        <v>-1.5</v>
+      </c>
+      <c r="M33">
+        <v>-0.5</v>
+      </c>
+      <c r="N33">
+        <v>-2</v>
+      </c>
+      <c r="O33">
+        <v>-0.5</v>
+      </c>
+      <c r="P33">
+        <v>1</v>
+      </c>
+      <c r="Q33">
+        <v>6.7</v>
+      </c>
+      <c r="R33">
+        <v>3.2</v>
+      </c>
+      <c r="S33">
+        <v>2.6</v>
+      </c>
+      <c r="V33">
+        <v>4.2</v>
+      </c>
+      <c r="W33">
+        <v>4.5</v>
+      </c>
+      <c r="X33">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34">
+        <v>3.3</v>
+      </c>
+      <c r="C34">
+        <v>3.15</v>
+      </c>
+      <c r="D34">
+        <v>3.15</v>
+      </c>
+      <c r="E34">
+        <v>3.15</v>
+      </c>
+      <c r="F34">
+        <v>3.15</v>
+      </c>
+      <c r="G34">
+        <v>3.375</v>
+      </c>
+      <c r="H34">
+        <v>3.375</v>
+      </c>
+      <c r="I34">
+        <v>3.375</v>
+      </c>
+      <c r="J34">
+        <v>3.375</v>
+      </c>
+      <c r="K34">
+        <v>3.375</v>
+      </c>
+      <c r="L34">
+        <v>0.7</v>
+      </c>
+      <c r="M34">
+        <v>1.8</v>
+      </c>
+      <c r="N34">
+        <v>0.8</v>
+      </c>
+      <c r="O34">
+        <v>1</v>
+      </c>
+      <c r="P34">
+        <v>1.5</v>
+      </c>
+      <c r="Q34">
+        <v>7</v>
+      </c>
+      <c r="R34">
+        <v>3.1</v>
+      </c>
+      <c r="S34">
+        <v>2.7</v>
+      </c>
+      <c r="T34">
+        <v>2.5</v>
+      </c>
+      <c r="U34">
+        <v>2.5</v>
+      </c>
+      <c r="V34">
+        <v>3.6</v>
+      </c>
+      <c r="W34">
+        <v>3.7</v>
+      </c>
+      <c r="X34">
+        <v>3.8</v>
+      </c>
+      <c r="Y34">
+        <v>3.9</v>
+      </c>
+      <c r="Z34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35">
+        <v>3.1</v>
+      </c>
+      <c r="C35">
+        <v>3</v>
+      </c>
+      <c r="D35">
+        <v>2.75</v>
+      </c>
+      <c r="G35">
+        <v>3.375</v>
+      </c>
+      <c r="H35">
+        <v>3.375</v>
+      </c>
+      <c r="I35">
+        <v>3.375</v>
+      </c>
+      <c r="L35">
+        <v>0.4</v>
+      </c>
+      <c r="M35">
+        <v>1.8</v>
+      </c>
+      <c r="N35">
+        <v>0.9</v>
+      </c>
+      <c r="O35">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P35">
+        <v>1.6</v>
+      </c>
+      <c r="Q35">
+        <v>7.2</v>
+      </c>
+      <c r="R35">
+        <v>4.7</v>
+      </c>
+      <c r="S35">
+        <v>2.9</v>
+      </c>
+      <c r="V35">
+        <v>3.9</v>
+      </c>
+      <c r="W35">
+        <v>4.5</v>
+      </c>
+      <c r="X35">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38">
+        <v>3</v>
+      </c>
+      <c r="C38">
+        <v>2.5</v>
+      </c>
+      <c r="D38">
+        <v>2</v>
+      </c>
+      <c r="E38">
+        <v>2</v>
+      </c>
+      <c r="F38">
+        <v>2</v>
+      </c>
+      <c r="G38">
+        <v>3.625</v>
+      </c>
+      <c r="H38">
+        <v>3.375</v>
+      </c>
+      <c r="I38">
+        <v>2.375</v>
+      </c>
+      <c r="J38">
+        <v>1.875</v>
+      </c>
+      <c r="K38">
+        <v>1.875</v>
+      </c>
+      <c r="L38">
+        <v>0.4</v>
+      </c>
+      <c r="M38">
+        <v>2.6</v>
+      </c>
+      <c r="N38">
+        <v>0.1</v>
+      </c>
+      <c r="O38">
+        <v>-1.5</v>
+      </c>
+      <c r="P38">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Q38">
+        <v>7.5</v>
+      </c>
+      <c r="R38">
+        <v>3.6</v>
+      </c>
+      <c r="S38">
+        <v>2.1</v>
+      </c>
+      <c r="T38">
+        <v>1.4</v>
+      </c>
+      <c r="U38">
+        <v>1.8</v>
+      </c>
+      <c r="V38">
+        <v>3.8</v>
+      </c>
+      <c r="W38">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="X38">
+        <v>4</v>
+      </c>
+      <c r="Y38">
+        <v>4</v>
+      </c>
+      <c r="Z38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>43</v>
+      </c>
+      <c r="B39">
+        <v>2.85</v>
+      </c>
+      <c r="C39">
+        <v>2.75</v>
+      </c>
+      <c r="D39">
+        <v>2.65</v>
+      </c>
+      <c r="E39">
+        <v>2.5</v>
+      </c>
+      <c r="F39">
+        <v>2.25</v>
+      </c>
+      <c r="G39">
+        <v>3.125</v>
+      </c>
+      <c r="H39">
+        <v>3.125</v>
+      </c>
+      <c r="I39">
+        <v>2.625</v>
+      </c>
+      <c r="J39">
+        <v>2.375</v>
+      </c>
+      <c r="K39">
+        <v>1.875</v>
+      </c>
+      <c r="L39">
+        <v>1.4</v>
+      </c>
+      <c r="M39">
+        <v>1.7</v>
+      </c>
+      <c r="N39">
+        <v>1.7</v>
+      </c>
+      <c r="O39">
+        <v>1.8</v>
+      </c>
+      <c r="P39">
+        <v>1.8</v>
+      </c>
+      <c r="Q39">
+        <v>7.6</v>
+      </c>
+      <c r="R39">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="S39">
+        <v>2.9</v>
+      </c>
+      <c r="T39">
+        <v>1.8</v>
+      </c>
+      <c r="U39">
+        <v>1.7</v>
+      </c>
+      <c r="V39">
+        <v>3.7</v>
+      </c>
+      <c r="W39">
+        <v>3.9</v>
+      </c>
+      <c r="X39">
+        <v>4.2</v>
+      </c>
+      <c r="Y39">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="Z39">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>44</v>
+      </c>
+      <c r="G40">
+        <v>3.375</v>
+      </c>
+      <c r="H40">
+        <v>3.875</v>
+      </c>
+      <c r="I40">
+        <v>3.875</v>
+      </c>
+      <c r="L40">
+        <v>0.8</v>
+      </c>
+      <c r="M40">
+        <v>0.5</v>
+      </c>
+      <c r="N40">
+        <v>-0.2</v>
+      </c>
+      <c r="O40">
+        <v>-0.4</v>
+      </c>
+      <c r="P40">
+        <v>0.4</v>
+      </c>
+      <c r="V40">
+        <v>3.6</v>
+      </c>
+      <c r="W40">
+        <v>3.7</v>
+      </c>
+      <c r="X40">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42">
+        <v>2.8</v>
+      </c>
+      <c r="C42">
+        <v>2.9</v>
+      </c>
+      <c r="D42">
+        <v>3</v>
+      </c>
+      <c r="G42">
+        <v>3.125</v>
+      </c>
+      <c r="H42">
+        <v>3.875</v>
+      </c>
+      <c r="I42">
+        <v>3.875</v>
+      </c>
+      <c r="J42">
+        <v>3.625</v>
+      </c>
+      <c r="L42">
+        <v>-1</v>
+      </c>
+      <c r="M42">
+        <v>0.5</v>
+      </c>
+      <c r="N42">
+        <v>0.5</v>
+      </c>
+      <c r="Q42">
+        <v>6.8</v>
+      </c>
+      <c r="R42">
+        <v>5.2</v>
+      </c>
+      <c r="S42">
+        <v>4</v>
+      </c>
+      <c r="V42">
+        <v>3.5</v>
+      </c>
+      <c r="W42">
+        <v>3.7</v>
+      </c>
+      <c r="X42">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>46</v>
+      </c>
+      <c r="G43">
+        <v>3.875</v>
+      </c>
+      <c r="H43">
+        <v>4.125</v>
+      </c>
+      <c r="I43">
+        <v>3.125</v>
+      </c>
+      <c r="J43">
+        <v>2.875</v>
+      </c>
+      <c r="K43">
+        <v>2.875</v>
+      </c>
+      <c r="L43">
+        <v>-2.1</v>
+      </c>
+      <c r="M43">
+        <v>0.9</v>
+      </c>
+      <c r="N43">
+        <v>1.3</v>
+      </c>
+      <c r="O43">
+        <v>1.4</v>
+      </c>
+      <c r="P43">
+        <v>1.7</v>
+      </c>
+      <c r="Q43">
+        <v>6.6</v>
+      </c>
+      <c r="R43">
+        <v>3.9</v>
+      </c>
+      <c r="S43">
+        <v>2.9</v>
+      </c>
+      <c r="T43">
+        <v>2.7</v>
+      </c>
+      <c r="U43">
+        <v>2.6</v>
+      </c>
+      <c r="V43">
+        <v>4</v>
+      </c>
+      <c r="W43">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="X43">
+        <v>4.5</v>
+      </c>
+      <c r="Y43">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="Z43">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>40</v>
+      </c>
+      <c r="B46">
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="C46">
+        <v>4.7699999999999996</v>
+      </c>
+      <c r="D46">
+        <v>4.59</v>
+      </c>
+      <c r="E46">
+        <v>4.41</v>
+      </c>
+      <c r="F46">
+        <v>4.05</v>
+      </c>
+      <c r="G46">
+        <v>3.125</v>
+      </c>
+      <c r="H46">
+        <v>4</v>
+      </c>
+      <c r="I46">
+        <v>3.875</v>
+      </c>
+      <c r="J46">
+        <v>3.75</v>
+      </c>
+      <c r="K46">
+        <v>3.375</v>
+      </c>
+      <c r="L46">
+        <v>-0.3</v>
+      </c>
+      <c r="M46">
+        <v>0.7</v>
+      </c>
+      <c r="N46">
+        <v>0.2</v>
+      </c>
+      <c r="O46">
+        <v>-1.5</v>
+      </c>
+      <c r="P46">
+        <v>-0.1</v>
+      </c>
+      <c r="Q46">
+        <v>4.5</v>
+      </c>
+      <c r="R46">
+        <v>3.8</v>
+      </c>
+      <c r="S46">
+        <v>2.6</v>
+      </c>
+      <c r="T46">
+        <v>2.4</v>
+      </c>
+      <c r="U46">
+        <v>2</v>
+      </c>
+      <c r="V46">
+        <v>3.8</v>
+      </c>
+      <c r="W46">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="X46">
+        <v>4.2</v>
+      </c>
+      <c r="Y46">
+        <v>4</v>
+      </c>
+      <c r="Z46">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47">
+        <v>4.7</v>
+      </c>
+      <c r="C47">
+        <v>4.8</v>
+      </c>
+      <c r="D47">
+        <v>5</v>
+      </c>
+      <c r="E47">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="F47">
+        <v>4.3</v>
+      </c>
+      <c r="G47">
+        <v>3.375</v>
+      </c>
+      <c r="H47">
+        <v>3.875</v>
+      </c>
+      <c r="I47">
+        <v>4.375</v>
+      </c>
+      <c r="J47">
+        <v>4.375</v>
+      </c>
+      <c r="K47">
+        <v>3.875</v>
+      </c>
+      <c r="L47">
+        <v>0.5</v>
+      </c>
+      <c r="M47">
+        <v>0.7</v>
+      </c>
+      <c r="N47">
+        <v>0.6</v>
+      </c>
+      <c r="O47">
+        <v>-0.2</v>
+      </c>
+      <c r="P47">
+        <v>-0.9</v>
+      </c>
+      <c r="Q47">
+        <v>6.9</v>
+      </c>
+      <c r="R47">
+        <v>3.7</v>
+      </c>
+      <c r="S47">
+        <v>2.7</v>
+      </c>
+      <c r="T47">
+        <v>2.4</v>
+      </c>
+      <c r="U47">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="V47">
+        <v>3.8</v>
+      </c>
+      <c r="W47">
+        <v>4.2</v>
+      </c>
+      <c r="X47">
+        <v>4.8</v>
+      </c>
+      <c r="Y47">
+        <v>5</v>
+      </c>
+      <c r="Z47">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>57</v>
+      </c>
+      <c r="B53">
+        <v>3.4</v>
+      </c>
+      <c r="C53">
+        <v>3.4</v>
+      </c>
+      <c r="D53">
+        <v>3.35</v>
+      </c>
+      <c r="E53">
+        <v>3.15</v>
+      </c>
+      <c r="F53">
+        <v>3</v>
+      </c>
+      <c r="G53">
+        <v>3.375</v>
+      </c>
+      <c r="H53">
+        <v>3.375</v>
+      </c>
+      <c r="I53">
+        <v>3.375</v>
+      </c>
+      <c r="J53">
+        <v>2.875</v>
+      </c>
+      <c r="K53">
+        <v>2.375</v>
+      </c>
+      <c r="L53">
+        <v>1.5</v>
+      </c>
+      <c r="M53">
+        <v>1</v>
+      </c>
+      <c r="N53">
+        <v>0.3</v>
+      </c>
+      <c r="O53">
+        <v>0.3</v>
+      </c>
+      <c r="P53">
+        <v>1.8</v>
+      </c>
+      <c r="Q53">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="R53">
+        <v>4.7</v>
+      </c>
+      <c r="S53">
+        <v>3.3</v>
+      </c>
+      <c r="T53">
+        <v>2.6</v>
+      </c>
+      <c r="U53">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="V53">
+        <v>3.9</v>
+      </c>
+      <c r="W53">
+        <v>4.3</v>
+      </c>
+      <c r="X53">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="Y53">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="Z53">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>104</v>
+      </c>
+      <c r="B54">
+        <v>2.94</v>
+      </c>
+      <c r="C54">
+        <v>2.94</v>
+      </c>
+      <c r="D54">
+        <v>3</v>
+      </c>
+      <c r="E54">
+        <v>3.05</v>
+      </c>
+      <c r="F54">
+        <v>3.08</v>
+      </c>
+      <c r="G54">
+        <v>3.375</v>
+      </c>
+      <c r="H54">
+        <v>3.375</v>
+      </c>
+      <c r="I54">
+        <v>3.375</v>
+      </c>
+      <c r="J54">
+        <v>3.125</v>
+      </c>
+      <c r="K54">
+        <v>2.625</v>
+      </c>
+      <c r="L54">
+        <v>-1.8</v>
+      </c>
+      <c r="M54">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="N54">
+        <v>1.7</v>
+      </c>
+      <c r="O54">
+        <v>1.4</v>
+      </c>
+      <c r="P54">
+        <v>1.5</v>
+      </c>
+      <c r="Q54">
+        <v>5.7</v>
+      </c>
+      <c r="R54">
+        <v>1.4</v>
+      </c>
+      <c r="S54">
+        <v>2</v>
+      </c>
+      <c r="T54">
+        <v>1.9</v>
+      </c>
+      <c r="U54">
+        <v>1.5</v>
+      </c>
+      <c r="V54">
+        <v>3.9</v>
+      </c>
+      <c r="W54">
+        <v>4.3</v>
+      </c>
+      <c r="X54">
+        <v>4.7</v>
+      </c>
+      <c r="Y54">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="Z54">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>59</v>
+      </c>
+      <c r="B55">
+        <v>3.5</v>
+      </c>
+      <c r="C55">
+        <v>3.5</v>
+      </c>
+      <c r="D55">
+        <v>3.5</v>
+      </c>
+      <c r="E55">
+        <v>3.25</v>
+      </c>
+      <c r="F55">
+        <v>3.25</v>
+      </c>
+      <c r="G55">
+        <v>3.375</v>
+      </c>
+      <c r="H55">
+        <v>3.625</v>
+      </c>
+      <c r="I55">
+        <v>3.625</v>
+      </c>
+      <c r="J55">
+        <v>3.375</v>
+      </c>
+      <c r="K55">
+        <v>3.125</v>
+      </c>
+      <c r="L55">
+        <v>0.2</v>
+      </c>
+      <c r="M55">
+        <v>1</v>
+      </c>
+      <c r="N55">
+        <v>1.5</v>
+      </c>
+      <c r="O55">
+        <v>1</v>
+      </c>
+      <c r="P55">
+        <v>2</v>
+      </c>
+      <c r="Q55">
+        <v>7</v>
+      </c>
+      <c r="R55">
+        <v>3.5</v>
+      </c>
+      <c r="S55">
+        <v>3</v>
+      </c>
+      <c r="T55">
+        <v>2.4</v>
+      </c>
+      <c r="U55">
+        <v>2</v>
+      </c>
+      <c r="V55">
+        <v>3.8</v>
+      </c>
+      <c r="W55">
+        <v>3.6</v>
+      </c>
+      <c r="X55">
+        <v>3.5</v>
+      </c>
+      <c r="Y55">
+        <v>3.5</v>
+      </c>
+      <c r="Z55">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>61</v>
+      </c>
+      <c r="B57">
+        <v>3.68</v>
+      </c>
+      <c r="C57">
+        <v>4.2</v>
+      </c>
+      <c r="D57">
+        <v>4.3</v>
+      </c>
+      <c r="E57">
+        <v>4.7</v>
+      </c>
+      <c r="F57">
+        <v>4.8</v>
+      </c>
+      <c r="G57">
+        <v>2.875</v>
+      </c>
+      <c r="H57">
+        <v>3.375</v>
+      </c>
+      <c r="I57">
+        <v>3.875</v>
+      </c>
+      <c r="J57">
+        <v>4.125</v>
+      </c>
+      <c r="K57">
+        <v>4.125</v>
+      </c>
+      <c r="L57">
+        <v>1.4</v>
+      </c>
+      <c r="M57">
+        <v>1</v>
+      </c>
+      <c r="N57">
+        <v>0.4</v>
+      </c>
+      <c r="O57">
+        <v>0.4</v>
+      </c>
+      <c r="P57">
+        <v>4</v>
+      </c>
+      <c r="Q57">
+        <v>3.6</v>
+      </c>
+      <c r="R57">
+        <v>3.6</v>
+      </c>
+      <c r="S57">
+        <v>4.8</v>
+      </c>
+      <c r="T57">
+        <v>3.7</v>
+      </c>
+      <c r="U57">
+        <v>3.7</v>
+      </c>
+      <c r="V57">
+        <v>4</v>
+      </c>
+      <c r="W57">
+        <v>4.3</v>
+      </c>
+      <c r="X57">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="Y57">
+        <v>4</v>
+      </c>
+      <c r="Z57">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>62</v>
+      </c>
+      <c r="B58">
+        <v>2.95</v>
+      </c>
+      <c r="C58">
+        <v>3.1</v>
+      </c>
+      <c r="D58">
+        <v>3.05</v>
+      </c>
+      <c r="E58">
+        <v>3.31</v>
+      </c>
+      <c r="F58">
+        <v>3.55</v>
+      </c>
+      <c r="G58">
+        <v>2.875</v>
+      </c>
+      <c r="H58">
+        <v>3</v>
+      </c>
+      <c r="I58">
+        <v>3.2</v>
+      </c>
+      <c r="J58">
+        <v>3.25</v>
+      </c>
+      <c r="K58">
+        <v>3.5</v>
+      </c>
+      <c r="L58">
+        <v>-1</v>
+      </c>
+      <c r="M58">
+        <v>0.9</v>
+      </c>
+      <c r="N58">
+        <v>1.4</v>
+      </c>
+      <c r="O58">
+        <v>1.8</v>
+      </c>
+      <c r="P58">
+        <v>1.9</v>
+      </c>
+      <c r="Q58">
+        <v>6.3</v>
+      </c>
+      <c r="R58">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="S58">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="T58">
+        <v>3.1</v>
+      </c>
+      <c r="U58">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="V58">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="W58">
+        <v>3.9</v>
+      </c>
+      <c r="X58">
+        <v>4</v>
+      </c>
+      <c r="Y58">
+        <v>3.9</v>
+      </c>
+      <c r="Z58">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>63</v>
+      </c>
+      <c r="B59">
+        <v>3.85</v>
+      </c>
+      <c r="C59">
+        <v>3.85</v>
+      </c>
+      <c r="D59">
+        <v>3.65</v>
+      </c>
+      <c r="G59">
+        <v>3.625</v>
+      </c>
+      <c r="H59">
+        <v>4.125</v>
+      </c>
+      <c r="I59">
+        <v>2.625</v>
+      </c>
+      <c r="J59">
+        <v>2.625</v>
+      </c>
+      <c r="K59">
+        <v>2.625</v>
+      </c>
+      <c r="L59">
+        <v>-0.6</v>
+      </c>
+      <c r="M59">
+        <v>2.8</v>
+      </c>
+      <c r="N59">
+        <v>1.8</v>
+      </c>
+      <c r="O59">
+        <v>1</v>
+      </c>
+      <c r="P59">
+        <v>0.3</v>
+      </c>
+      <c r="Q59">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="R59">
+        <v>5.3</v>
+      </c>
+      <c r="S59">
+        <v>3.9</v>
+      </c>
+      <c r="T59">
+        <v>3.3</v>
+      </c>
+      <c r="U59">
+        <v>2.9</v>
+      </c>
+      <c r="V59">
+        <v>3.6</v>
+      </c>
+      <c r="W59">
+        <v>4.2</v>
+      </c>
+      <c r="X59">
+        <v>5.5</v>
+      </c>
+      <c r="Y59">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="Z59">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>64</v>
+      </c>
+      <c r="B60">
+        <v>2.95</v>
+      </c>
+      <c r="C60">
+        <v>3.2</v>
+      </c>
+      <c r="D60">
+        <v>3.5</v>
+      </c>
+      <c r="E60">
+        <v>3.6</v>
+      </c>
+      <c r="F60">
+        <v>3.75</v>
+      </c>
+      <c r="G60">
+        <v>3.125</v>
+      </c>
+      <c r="H60">
+        <v>3.375</v>
+      </c>
+      <c r="I60">
+        <v>3.875</v>
+      </c>
+      <c r="J60">
+        <v>4.125</v>
+      </c>
+      <c r="K60">
+        <v>4.375</v>
+      </c>
+      <c r="L60">
+        <v>-1</v>
+      </c>
+      <c r="M60">
+        <v>5</v>
+      </c>
+      <c r="N60">
+        <v>2</v>
+      </c>
+      <c r="O60">
+        <v>2</v>
+      </c>
+      <c r="P60">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="Q60">
+        <v>6.7</v>
+      </c>
+      <c r="R60">
+        <v>1.5</v>
+      </c>
+      <c r="S60">
+        <v>0</v>
+      </c>
+      <c r="T60">
+        <v>2</v>
+      </c>
+      <c r="U60">
+        <v>2</v>
+      </c>
+      <c r="V60">
+        <v>3.5</v>
+      </c>
+      <c r="W60">
+        <v>3.6</v>
+      </c>
+      <c r="X60">
+        <v>3.7</v>
+      </c>
+      <c r="Y60">
+        <v>3.5</v>
+      </c>
+      <c r="Z60">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>65</v>
+      </c>
+      <c r="B61">
+        <v>3.75</v>
+      </c>
+      <c r="C61">
+        <v>4.12</v>
+      </c>
+      <c r="D61">
+        <v>4.45</v>
+      </c>
+      <c r="E61">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="F61">
+        <v>3.85</v>
+      </c>
+      <c r="G61">
+        <v>3.37</v>
+      </c>
+      <c r="H61">
+        <v>3.87</v>
+      </c>
+      <c r="I61">
+        <v>4.37</v>
+      </c>
+      <c r="J61">
+        <v>4.37</v>
+      </c>
+      <c r="K61">
+        <v>3.87</v>
+      </c>
+      <c r="L61">
+        <v>2.5</v>
+      </c>
+      <c r="M61">
+        <v>3.2</v>
+      </c>
+      <c r="N61">
+        <v>3.5</v>
+      </c>
+      <c r="O61">
+        <v>2.1</v>
+      </c>
+      <c r="P61">
+        <v>1.9</v>
+      </c>
+      <c r="Q61">
+        <v>6.8</v>
+      </c>
+      <c r="R61">
+        <v>6.1</v>
+      </c>
+      <c r="S61">
+        <v>5.3</v>
+      </c>
+      <c r="T61">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="U61">
+        <v>3.2</v>
+      </c>
+      <c r="V61">
+        <v>3.8</v>
+      </c>
+      <c r="W61">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="X61">
+        <v>4.3</v>
+      </c>
+      <c r="Y61">
+        <v>4.8</v>
+      </c>
+      <c r="Z61">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>66</v>
+      </c>
+      <c r="B62">
+        <v>3.09</v>
+      </c>
+      <c r="C62">
+        <v>3.18</v>
+      </c>
+      <c r="D62">
+        <v>2.93</v>
+      </c>
+      <c r="E62">
+        <v>2.75</v>
+      </c>
+      <c r="F62">
+        <v>2.58</v>
+      </c>
+      <c r="G62">
+        <v>3.375</v>
+      </c>
+      <c r="H62">
+        <v>3.125</v>
+      </c>
+      <c r="I62">
+        <v>2.625</v>
+      </c>
+      <c r="J62">
+        <v>2.375</v>
+      </c>
+      <c r="K62">
+        <v>2.375</v>
+      </c>
+      <c r="L62">
+        <v>1.9</v>
+      </c>
+      <c r="M62">
+        <v>3.5</v>
+      </c>
+      <c r="N62">
+        <v>3.6</v>
+      </c>
+      <c r="O62">
+        <v>3.5</v>
+      </c>
+      <c r="P62">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="Q62">
+        <v>4.2</v>
+      </c>
+      <c r="R62">
+        <v>3.5</v>
+      </c>
+      <c r="S62">
+        <v>2.8</v>
+      </c>
+      <c r="T62">
+        <v>2.5</v>
+      </c>
+      <c r="U62">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="V62">
+        <v>3.5</v>
+      </c>
+      <c r="W62">
+        <v>3.3</v>
+      </c>
+      <c r="X62">
+        <v>3.1</v>
+      </c>
+      <c r="Y62">
+        <v>3</v>
+      </c>
+      <c r="Z62">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>67</v>
+      </c>
+      <c r="B63">
+        <v>2.8</v>
+      </c>
+      <c r="C63">
+        <v>2.7</v>
+      </c>
+      <c r="D63">
+        <v>2.6</v>
+      </c>
+      <c r="E63">
+        <v>2.5</v>
+      </c>
+      <c r="F63">
+        <v>2.4</v>
+      </c>
+      <c r="G63">
+        <v>2.625</v>
+      </c>
+      <c r="H63">
+        <v>2.625</v>
+      </c>
+      <c r="I63">
+        <v>2.375</v>
+      </c>
+      <c r="J63">
+        <v>2.125</v>
+      </c>
+      <c r="K63">
+        <v>1.625</v>
+      </c>
+      <c r="L63">
+        <v>-0.3</v>
+      </c>
+      <c r="M63">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="N63">
+        <v>-0.8</v>
+      </c>
+      <c r="O63">
+        <v>-0.1</v>
+      </c>
+      <c r="P63">
+        <v>-0.1</v>
+      </c>
+      <c r="Q63">
+        <v>7.7</v>
+      </c>
+      <c r="R63">
+        <v>5</v>
+      </c>
+      <c r="S63">
+        <v>3</v>
+      </c>
+      <c r="T63">
+        <v>1.8</v>
+      </c>
+      <c r="U63">
+        <v>1.5</v>
+      </c>
+      <c r="V63">
+        <v>4.3</v>
+      </c>
+      <c r="W63">
+        <v>5.2</v>
+      </c>
+      <c r="X63">
+        <v>6</v>
+      </c>
+      <c r="Y63">
+        <v>6.4</v>
+      </c>
+      <c r="Z63">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>68</v>
+      </c>
+      <c r="B64">
+        <v>3.25</v>
+      </c>
+      <c r="C64">
+        <v>3.5</v>
+      </c>
+      <c r="D64">
+        <v>3.75</v>
+      </c>
+      <c r="E64">
+        <v>4</v>
+      </c>
+      <c r="F64">
+        <v>4.25</v>
+      </c>
+      <c r="G64">
+        <v>3.375</v>
+      </c>
+      <c r="H64">
+        <v>3.875</v>
+      </c>
+      <c r="I64">
+        <v>4.125</v>
+      </c>
+      <c r="J64">
+        <v>4.375</v>
+      </c>
+      <c r="K64">
+        <v>4.625</v>
+      </c>
+      <c r="L64">
+        <v>-1</v>
+      </c>
+      <c r="M64">
+        <v>1.5</v>
+      </c>
+      <c r="N64">
+        <v>2.5</v>
+      </c>
+      <c r="O64">
+        <v>2.7</v>
+      </c>
+      <c r="P64">
+        <v>2.4</v>
+      </c>
+      <c r="Q64">
+        <v>8.5</v>
+      </c>
+      <c r="R64">
+        <v>5.5</v>
+      </c>
+      <c r="S64">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="T64">
+        <v>5</v>
+      </c>
+      <c r="U64">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="V64">
+        <v>4</v>
+      </c>
+      <c r="W64">
+        <v>4.2</v>
+      </c>
+      <c r="X64">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="Y64">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="Z64">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>69</v>
+      </c>
+      <c r="B65">
+        <v>3.9</v>
+      </c>
+      <c r="C65">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="D65">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="E65">
+        <v>4.2</v>
+      </c>
+      <c r="F65">
+        <v>3.9</v>
+      </c>
+      <c r="G65">
+        <v>3.625</v>
+      </c>
+      <c r="H65">
+        <v>4.625</v>
+      </c>
+      <c r="I65">
+        <v>4.625</v>
+      </c>
+      <c r="J65">
+        <v>4.625</v>
+      </c>
+      <c r="K65">
+        <v>3.625</v>
+      </c>
+      <c r="L65">
+        <v>2</v>
+      </c>
+      <c r="M65">
+        <v>4</v>
+      </c>
+      <c r="N65">
+        <v>3.2</v>
+      </c>
+      <c r="O65">
+        <v>2.8</v>
+      </c>
+      <c r="P65">
+        <v>2.7</v>
+      </c>
+      <c r="Q65">
+        <v>7.6</v>
+      </c>
+      <c r="R65">
+        <v>4.2</v>
+      </c>
+      <c r="S65">
+        <v>3.6</v>
+      </c>
+      <c r="T65">
+        <v>3</v>
+      </c>
+      <c r="U65">
+        <v>2.6</v>
+      </c>
+      <c r="V65">
+        <v>3.3</v>
+      </c>
+      <c r="W65">
+        <v>3.1</v>
+      </c>
+      <c r="X65">
+        <v>3.1</v>
+      </c>
+      <c r="Y65">
+        <v>3.2</v>
+      </c>
+      <c r="Z65">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>70</v>
+      </c>
+      <c r="B66">
+        <v>2.9</v>
+      </c>
+      <c r="C66">
+        <v>2.7</v>
+      </c>
+      <c r="D66">
+        <v>2.5</v>
+      </c>
+      <c r="E66">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F66">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G66">
+        <v>2.13</v>
+      </c>
+      <c r="H66">
+        <v>1.88</v>
+      </c>
+      <c r="I66">
+        <v>1.88</v>
+      </c>
+      <c r="J66">
+        <v>1.65</v>
+      </c>
+      <c r="K66">
+        <v>1.65</v>
+      </c>
+      <c r="L66">
+        <v>-2.7</v>
+      </c>
+      <c r="M66">
+        <v>0.9</v>
+      </c>
+      <c r="N66">
+        <v>1.9</v>
+      </c>
+      <c r="O66">
+        <v>1</v>
+      </c>
+      <c r="P66">
+        <v>2.7</v>
+      </c>
+      <c r="Q66">
+        <v>5.7</v>
+      </c>
+      <c r="R66">
+        <v>3</v>
+      </c>
+      <c r="S66">
+        <v>2.7</v>
+      </c>
+      <c r="T66">
+        <v>2.5</v>
+      </c>
+      <c r="U66">
+        <v>2.6</v>
+      </c>
+      <c r="V66">
+        <v>3.7</v>
+      </c>
+      <c r="W66">
+        <v>3.4</v>
+      </c>
+      <c r="X66">
+        <v>3.3</v>
+      </c>
+      <c r="Y66">
+        <v>3.4</v>
+      </c>
+      <c r="Z66">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>89</v>
+      </c>
+      <c r="B68">
+        <v>3.45</v>
+      </c>
+      <c r="C68">
+        <v>3.7</v>
+      </c>
+      <c r="D68">
+        <v>3.75</v>
+      </c>
+      <c r="E68">
+        <v>3.55</v>
+      </c>
+      <c r="F68">
+        <v>3.4</v>
+      </c>
+      <c r="G68">
+        <v>3.125</v>
+      </c>
+      <c r="H68">
+        <v>3.625</v>
+      </c>
+      <c r="I68">
+        <v>3.375</v>
+      </c>
+      <c r="J68">
+        <v>2.875</v>
+      </c>
+      <c r="K68">
+        <v>2.625</v>
+      </c>
+      <c r="L68">
+        <v>1.5</v>
+      </c>
+      <c r="M68">
+        <v>2</v>
+      </c>
+      <c r="N68">
+        <v>1.7</v>
+      </c>
+      <c r="O68">
+        <v>1.4</v>
+      </c>
+      <c r="P68">
+        <v>1.4</v>
+      </c>
+      <c r="Q68">
+        <v>7.8</v>
+      </c>
+      <c r="R68">
+        <v>4.8</v>
+      </c>
+      <c r="S68">
+        <v>3.5</v>
+      </c>
+      <c r="T68">
+        <v>2.8</v>
+      </c>
+      <c r="U68">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="V68">
+        <v>3.8</v>
+      </c>
+      <c r="W68">
+        <v>4</v>
+      </c>
+      <c r="X68">
+        <v>4.3</v>
+      </c>
+      <c r="Y68">
+        <v>4</v>
+      </c>
+      <c r="Z68">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>90</v>
+      </c>
+      <c r="B69">
+        <v>3</v>
+      </c>
+      <c r="C69">
+        <v>3.3</v>
+      </c>
+      <c r="D69">
+        <v>2.9</v>
+      </c>
+      <c r="E69">
+        <v>2.8</v>
+      </c>
+      <c r="F69">
+        <v>2.7</v>
+      </c>
+      <c r="G69">
+        <v>3.375</v>
+      </c>
+      <c r="H69">
+        <v>3.875</v>
+      </c>
+      <c r="I69">
+        <v>2.875</v>
+      </c>
+      <c r="J69">
+        <v>1.375</v>
+      </c>
+      <c r="K69">
+        <v>1.125</v>
+      </c>
+      <c r="L69">
+        <v>-1.7</v>
+      </c>
+      <c r="M69">
+        <v>0.9</v>
+      </c>
+      <c r="N69">
+        <v>0.2</v>
+      </c>
+      <c r="O69">
+        <v>0.5</v>
+      </c>
+      <c r="P69">
+        <v>1.6</v>
+      </c>
+      <c r="Q69">
+        <v>6.6</v>
+      </c>
+      <c r="R69">
+        <v>3.5</v>
+      </c>
+      <c r="S69">
+        <v>2</v>
+      </c>
+      <c r="T69">
+        <v>1.9</v>
+      </c>
+      <c r="U69">
+        <v>2</v>
+      </c>
+      <c r="V69">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="W69">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="X69">
+        <v>5.8</v>
+      </c>
+      <c r="Y69">
+        <v>5.8</v>
+      </c>
+      <c r="Z69">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>75</v>
+      </c>
+      <c r="B70">
+        <v>3.65</v>
+      </c>
+      <c r="C70">
+        <v>4.25</v>
+      </c>
+      <c r="D70">
+        <v>4.25</v>
+      </c>
+      <c r="E70">
+        <v>3.75</v>
+      </c>
+      <c r="F70">
+        <v>3.25</v>
+      </c>
+      <c r="G70">
+        <v>3.625</v>
+      </c>
+      <c r="H70">
+        <v>3.875</v>
+      </c>
+      <c r="I70">
+        <v>3.875</v>
+      </c>
+      <c r="J70">
+        <v>3.375</v>
+      </c>
+      <c r="K70">
+        <v>2.875</v>
+      </c>
+      <c r="L70">
+        <v>0.8</v>
+      </c>
+      <c r="M70">
+        <v>1.6</v>
+      </c>
+      <c r="N70">
+        <v>1.7</v>
+      </c>
+      <c r="O70">
+        <v>1.4</v>
+      </c>
+      <c r="P70">
+        <v>1.4</v>
+      </c>
+      <c r="Q70">
+        <v>7.2</v>
+      </c>
+      <c r="R70">
+        <v>3.8</v>
+      </c>
+      <c r="S70">
+        <v>2.5</v>
+      </c>
+      <c r="T70">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="U70">
+        <v>2</v>
+      </c>
+      <c r="V70">
+        <v>3.7</v>
+      </c>
+      <c r="W70">
+        <v>3.8</v>
+      </c>
+      <c r="X70">
+        <v>3.9</v>
+      </c>
+      <c r="Y70">
+        <v>3.8</v>
+      </c>
+      <c r="Z70">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>76</v>
+      </c>
+      <c r="B71">
+        <v>3.66</v>
+      </c>
+      <c r="C71">
+        <v>3.92</v>
+      </c>
+      <c r="D71">
+        <v>4.22</v>
+      </c>
+      <c r="E71">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="F71">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="G71">
+        <v>2.375</v>
+      </c>
+      <c r="H71">
+        <v>3.125</v>
+      </c>
+      <c r="I71">
+        <v>3.375</v>
+      </c>
+      <c r="J71">
+        <v>3.625</v>
+      </c>
+      <c r="K71">
+        <v>4.125</v>
+      </c>
+      <c r="L71">
+        <v>2.4</v>
+      </c>
+      <c r="M71">
+        <v>2.5</v>
+      </c>
+      <c r="N71">
+        <v>1.6</v>
+      </c>
+      <c r="O71">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="P71">
+        <v>1.5</v>
+      </c>
+      <c r="Q71">
+        <v>7.6</v>
+      </c>
+      <c r="R71">
+        <v>5.4</v>
+      </c>
+      <c r="S71">
+        <v>4.5</v>
+      </c>
+      <c r="T71">
+        <v>4.3</v>
+      </c>
+      <c r="U71">
+        <v>4</v>
+      </c>
+      <c r="V71">
+        <v>3.5</v>
+      </c>
+      <c r="W71">
+        <v>3.6</v>
+      </c>
+      <c r="X71">
+        <v>3.8</v>
+      </c>
+      <c r="Y71">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="Z71">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>77</v>
+      </c>
+      <c r="B72">
+        <v>3</v>
+      </c>
+      <c r="G72">
+        <v>3</v>
+      </c>
+      <c r="H72">
+        <v>3.25</v>
+      </c>
+      <c r="Q72">
+        <v>5.5</v>
+      </c>
+      <c r="V72">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>9</v>
+      </c>
+      <c r="B73">
+        <v>2.65</v>
+      </c>
+      <c r="C73">
+        <v>1.85</v>
+      </c>
+      <c r="D73">
+        <v>1.7</v>
+      </c>
+      <c r="G73">
+        <v>3.375</v>
+      </c>
+      <c r="H73">
+        <v>3.625</v>
+      </c>
+      <c r="I73">
+        <v>2.875</v>
+      </c>
+      <c r="J73">
+        <v>1.875</v>
+      </c>
+      <c r="K73">
+        <v>0.875</v>
+      </c>
+      <c r="L73">
+        <v>-0.2</v>
+      </c>
+      <c r="M73">
+        <v>0.4</v>
+      </c>
+      <c r="N73">
+        <v>-1.4</v>
+      </c>
+      <c r="O73">
+        <v>-1.6</v>
+      </c>
+      <c r="P73">
+        <v>-1.6</v>
+      </c>
+      <c r="Q73">
+        <v>7.4</v>
+      </c>
+      <c r="R73">
+        <v>3.5</v>
+      </c>
+      <c r="S73">
+        <v>2.7</v>
+      </c>
+      <c r="T73">
+        <v>2.1</v>
+      </c>
+      <c r="U73">
+        <v>1.6</v>
+      </c>
+      <c r="V73">
+        <v>3.5</v>
+      </c>
+      <c r="W73">
+        <v>4.3</v>
+      </c>
+      <c r="X73">
+        <v>5.2</v>
+      </c>
+      <c r="Y73">
+        <v>5.6</v>
+      </c>
+      <c r="Z73">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="74" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>78</v>
+      </c>
+      <c r="B74">
+        <v>2.95</v>
+      </c>
+      <c r="C74">
+        <v>2.95</v>
+      </c>
+      <c r="D74">
+        <v>2.8</v>
+      </c>
+      <c r="G74">
+        <v>3.625</v>
+      </c>
+      <c r="H74">
+        <v>3.625</v>
+      </c>
+      <c r="I74">
+        <v>3.625</v>
+      </c>
+      <c r="L74">
+        <v>1.6</v>
+      </c>
+      <c r="M74">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="N74">
+        <v>1.9</v>
+      </c>
+      <c r="O74">
+        <v>1.5</v>
+      </c>
+      <c r="P74">
+        <v>1</v>
+      </c>
+      <c r="Q74">
+        <v>7.6</v>
+      </c>
+      <c r="R74">
+        <v>4</v>
+      </c>
+      <c r="S74">
+        <v>3.6</v>
+      </c>
+      <c r="V74">
+        <v>3.4</v>
+      </c>
+      <c r="W74">
+        <v>3.5</v>
+      </c>
+      <c r="X74">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="75" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>79</v>
+      </c>
+      <c r="B75">
+        <v>2.9</v>
+      </c>
+      <c r="C75">
+        <v>2.5</v>
+      </c>
+      <c r="D75">
+        <v>2.25</v>
+      </c>
+      <c r="E75">
+        <v>2.5</v>
+      </c>
+      <c r="F75">
+        <v>2.5</v>
+      </c>
+      <c r="G75">
+        <v>3.375</v>
+      </c>
+      <c r="H75">
+        <v>3.375</v>
+      </c>
+      <c r="I75">
+        <v>2.875</v>
+      </c>
+      <c r="J75">
+        <v>2.375</v>
+      </c>
+      <c r="K75">
+        <v>2.375</v>
+      </c>
+      <c r="L75">
+        <v>-0.5</v>
+      </c>
+      <c r="M75">
+        <v>1.4</v>
+      </c>
+      <c r="N75">
+        <v>1.4</v>
+      </c>
+      <c r="O75">
+        <v>-1.6</v>
+      </c>
+      <c r="P75">
+        <v>-2</v>
+      </c>
+      <c r="Q75">
+        <v>7</v>
+      </c>
+      <c r="R75">
+        <v>4.5</v>
+      </c>
+      <c r="S75">
+        <v>4</v>
+      </c>
+      <c r="T75">
+        <v>3</v>
+      </c>
+      <c r="U75">
+        <v>2.7</v>
+      </c>
+      <c r="V75">
+        <v>3.9</v>
+      </c>
+      <c r="W75">
+        <v>4.7</v>
+      </c>
+      <c r="X75">
+        <v>5.3</v>
+      </c>
+      <c r="Y75">
+        <v>5.5</v>
+      </c>
+      <c r="Z75">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>80</v>
+      </c>
+      <c r="B76">
+        <v>3.15</v>
+      </c>
+      <c r="C76">
+        <v>3.25</v>
+      </c>
+      <c r="D76">
+        <v>3.35</v>
+      </c>
+      <c r="G76">
+        <v>3.625</v>
+      </c>
+      <c r="H76">
+        <v>3.875</v>
+      </c>
+      <c r="I76">
+        <v>3.875</v>
+      </c>
+      <c r="L76">
+        <v>1.5</v>
+      </c>
+      <c r="M76">
+        <v>2</v>
+      </c>
+      <c r="N76">
+        <v>1</v>
+      </c>
+      <c r="O76">
+        <v>1.5</v>
+      </c>
+      <c r="P76">
+        <v>1</v>
+      </c>
+      <c r="Q76">
+        <v>7</v>
+      </c>
+      <c r="R76">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="S76">
+        <v>5</v>
+      </c>
+      <c r="V76">
+        <v>3.6</v>
+      </c>
+      <c r="W76">
+        <v>3.8</v>
+      </c>
+      <c r="X76">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="77" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>81</v>
+      </c>
+      <c r="B77">
+        <v>3.3</v>
+      </c>
+      <c r="C77">
+        <v>3.5</v>
+      </c>
+      <c r="D77">
+        <v>3.5</v>
+      </c>
+      <c r="E77">
+        <v>3.6</v>
+      </c>
+      <c r="F77">
+        <v>3.6</v>
+      </c>
+      <c r="G77">
+        <v>3.375</v>
+      </c>
+      <c r="H77">
+        <v>3.625</v>
+      </c>
+      <c r="I77">
+        <v>3.625</v>
+      </c>
+      <c r="J77">
+        <v>3.125</v>
+      </c>
+      <c r="K77">
+        <v>2.875</v>
+      </c>
+      <c r="L77">
+        <v>0.8</v>
+      </c>
+      <c r="M77">
+        <v>1.5</v>
+      </c>
+      <c r="N77">
+        <v>1.8</v>
+      </c>
+      <c r="O77">
+        <v>1.8</v>
+      </c>
+      <c r="P77">
+        <v>1.8</v>
+      </c>
+      <c r="Q77">
+        <v>7.2</v>
+      </c>
+      <c r="R77">
+        <v>5.6</v>
+      </c>
+      <c r="S77">
+        <v>5.2</v>
+      </c>
+      <c r="T77">
+        <v>4.7</v>
+      </c>
+      <c r="U77">
+        <v>3.5</v>
+      </c>
+      <c r="V77">
+        <v>3.7</v>
+      </c>
+      <c r="W77">
+        <v>3.8</v>
+      </c>
+      <c r="X77">
+        <v>3.9</v>
+      </c>
+      <c r="Y77">
+        <v>4</v>
+      </c>
+      <c r="Z77">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>82</v>
+      </c>
+      <c r="B78">
+        <v>3.5</v>
+      </c>
+      <c r="C78">
+        <v>3.05</v>
+      </c>
+      <c r="G78">
+        <v>3.625</v>
+      </c>
+      <c r="H78">
+        <v>3.625</v>
+      </c>
+      <c r="I78">
+        <v>3.625</v>
+      </c>
+      <c r="L78">
+        <v>0.1</v>
+      </c>
+      <c r="M78">
+        <v>2.6</v>
+      </c>
+      <c r="N78">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="O78">
+        <v>1.4</v>
+      </c>
+      <c r="P78">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Q78">
+        <v>6.9</v>
+      </c>
+      <c r="R78">
+        <v>3</v>
+      </c>
+      <c r="S78">
+        <v>1.6</v>
+      </c>
+      <c r="V78">
+        <v>3.6</v>
+      </c>
+      <c r="W78">
+        <v>3.6</v>
+      </c>
+      <c r="X78">
+        <v>3.8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>